<commit_message>
Changes for approve-reject-flow prototype
</commit_message>
<xml_diff>
--- a/UX-test/approve-reject/flow-test-tasks.xlsx
+++ b/UX-test/approve-reject/flow-test-tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylmejia/Documents/repos/repo-sketch-cactus/master/design-system/UX-test/approve-reject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylmejia/Documents/Repo/design-system/design-system/UX-test/approve-reject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9CB612-A6B1-4244-AFA9-CD5FFA3D06C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D373CC-A70F-EC4F-A4B1-BE20E50A8855}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14640" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="15620" windowHeight="14640" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -246,30 +246,15 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -286,6 +271,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -305,7 +305,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -604,7 +604,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,67 +614,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="10" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="10" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="7">
         <v>3</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change names on the files on the test
</commit_message>
<xml_diff>
--- a/UX-test/approve-reject/flow-test-tasks.xlsx
+++ b/UX-test/approve-reject/flow-test-tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylmejia/Documents/Repo/design-system/design-system/UX-test/approve-reject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D373CC-A70F-EC4F-A4B1-BE20E50A8855}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEF2BFE-9FCF-3A4F-AB90-2A808859420A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="15620" windowHeight="14640" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
   </bookViews>
@@ -245,9 +245,6 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -271,6 +268,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -604,7 +604,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,13 +621,13 @@
       <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -638,43 +638,43 @@
       <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create a general prototype for test
Create a general prototype for test
Create a general script for test
Little changes on prorotypes of assets and general flow to organized for the general prototype
</commit_message>
<xml_diff>
--- a/UX-test/approve-reject/flow-test-tasks.xlsx
+++ b/UX-test/approve-reject/flow-test-tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylmejia/Documents/Repo/design-system/design-system/UX-test/approve-reject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylmejia/Documents/repos/repo-sketch-cactus/master/design-system/UX-test/approve-reject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEF2BFE-9FCF-3A4F-AB90-2A808859420A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EC9354-6994-0C45-B901-1F99EBBC9EB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="15620" windowHeight="14640" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="14600" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Tasks</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Number of people who reject the asset:</t>
   </si>
   <si>
-    <t>Flow-test Start on Dashboard page</t>
+    <t>Name: GeneralFlow-test Start on Dashboard page</t>
   </si>
 </sst>
 </file>
@@ -104,7 +104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -239,11 +239,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -286,6 +297,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -305,7 +319,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -601,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657FE3D-C789-FA47-A22F-70453D6154E9}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,76 +627,90 @@
     <col min="3" max="3" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="14"/>
     </row>
-    <row r="2" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
+    <row r="5" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="4" t="s">
+    <row r="6" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="4" t="s">
+    <row r="7" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+    <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+    <row r="9" spans="1:3" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A3:A5"/>
+  <mergeCells count="5">
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>